<commit_message>
Byocitin clustering with reduced features
</commit_message>
<xml_diff>
--- a/inventory-biocytin-raw-29-electrophydata-regressionclasses.xlsx
+++ b/inventory-biocytin-raw-29-electrophydata-regressionclasses.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="0" windowWidth="14625" windowHeight="5085" tabRatio="616" activeTab="1"/>
+    <workbookView minimized="1" xWindow="5580" yWindow="0" windowWidth="13620" windowHeight="5085" tabRatio="616"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="13" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1408" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1411" uniqueCount="212">
   <si>
     <t>CTIP2-manual</t>
   </si>
@@ -666,6 +666,12 @@
   <si>
     <t>Cluster-size</t>
   </si>
+  <si>
+    <t>double</t>
+  </si>
+  <si>
+    <t>single</t>
+  </si>
 </sst>
 </file>
 
@@ -939,6 +945,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1213,11 +1220,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1434361680"/>
-        <c:axId val="-1434356240"/>
+        <c:axId val="-1909126304"/>
+        <c:axId val="-1909136640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1434361680"/>
+        <c:axId val="-1909126304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1274,12 +1281,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1434356240"/>
+        <c:crossAx val="-1909136640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1434356240"/>
+        <c:axId val="-1909136640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1336,7 +1343,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1434361680"/>
+        <c:crossAx val="-1909126304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1425,6 +1432,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1490,98 +1498,35 @@
               <c:f>'Clustering and Depth'!$E$3:$E$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="30">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -1592,98 +1537,35 @@
               <c:f>'Clustering and Depth'!$G$3:$G$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="31"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="30">
                   <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
@@ -1699,11 +1581,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1434357328"/>
-        <c:axId val="-1434355696"/>
+        <c:axId val="-1909135008"/>
+        <c:axId val="-1909133376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1434357328"/>
+        <c:axId val="-1909135008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1760,12 +1642,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1434355696"/>
+        <c:crossAx val="-1909133376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1434355696"/>
+        <c:axId val="-1909133376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1822,7 +1704,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1434357328"/>
+        <c:crossAx val="-1909135008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3338,9 +3220,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BK146"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
+      <selection pane="bottomLeft" activeCell="AI5" sqref="AI5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10754,11 +10636,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BM43"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:BM47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="AD1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AJ44" sqref="AJ44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10776,14 +10659,13 @@
     <col min="14" max="16" width="13" style="7" hidden="1" customWidth="1"/>
     <col min="17" max="29" width="9.140625" style="7" hidden="1" customWidth="1"/>
     <col min="30" max="30" width="9.140625" style="7" customWidth="1"/>
-    <col min="31" max="31" width="14.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14.85546875" style="7" customWidth="1"/>
     <col min="32" max="34" width="9.140625" style="7" customWidth="1"/>
-    <col min="35" max="35" width="12.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="36" max="37" width="12.42578125" style="7" customWidth="1"/>
-    <col min="38" max="41" width="10.28515625" style="7" hidden="1" customWidth="1"/>
-    <col min="42" max="44" width="10.28515625" style="6" hidden="1" customWidth="1"/>
-    <col min="45" max="45" width="9.42578125" style="6" hidden="1" customWidth="1"/>
-    <col min="46" max="65" width="0" style="6" hidden="1" customWidth="1"/>
+    <col min="35" max="37" width="12.42578125" style="7" customWidth="1"/>
+    <col min="38" max="41" width="10.28515625" style="7" customWidth="1"/>
+    <col min="42" max="44" width="10.28515625" style="6" customWidth="1"/>
+    <col min="45" max="45" width="9.42578125" style="6" customWidth="1"/>
+    <col min="46" max="65" width="8.85546875" style="6" customWidth="1"/>
     <col min="66" max="16384" width="8.85546875" style="7"/>
   </cols>
   <sheetData>
@@ -10984,7 +10866,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:65" hidden="1" x14ac:dyDescent="0.25">
       <c r="E2" s="6" t="s">
         <v>115</v>
       </c>
@@ -11082,7 +10964,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:65" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>92</v>
       </c>
@@ -11193,6 +11075,9 @@
         <f>SUM(AP3:AS3)</f>
         <v>14</v>
       </c>
+      <c r="AJ3">
+        <v>1</v>
+      </c>
       <c r="AK3">
         <v>1</v>
       </c>
@@ -11271,7 +11156,7 @@
         <v>62.12139892578125</v>
       </c>
     </row>
-    <row r="4" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:65" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>92</v>
       </c>
@@ -11380,6 +11265,9 @@
       <c r="AI4" s="7">
         <f t="shared" ref="AI4:AI27" si="4">SUM(AP4:AS4)</f>
         <v>8</v>
+      </c>
+      <c r="AJ4">
+        <v>2</v>
       </c>
       <c r="AK4">
         <v>2</v>
@@ -11556,6 +11444,9 @@
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
+      <c r="AJ5">
+        <v>2</v>
+      </c>
       <c r="AK5">
         <v>2</v>
       </c>
@@ -11614,7 +11505,7 @@
       <c r="BB5" s="19"/>
       <c r="BC5" s="19"/>
     </row>
-    <row r="6" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:65" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>92</v>
       </c>
@@ -11725,6 +11616,9 @@
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
+      <c r="AJ6">
+        <v>2</v>
+      </c>
       <c r="AK6">
         <v>2</v>
       </c>
@@ -11788,7 +11682,7 @@
         <v>117.59999847412109</v>
       </c>
     </row>
-    <row r="7" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:65" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>92</v>
       </c>
@@ -11898,6 +11792,9 @@
       <c r="AI7" s="7">
         <f t="shared" si="4"/>
         <v>9</v>
+      </c>
+      <c r="AJ7">
+        <v>2</v>
       </c>
       <c r="AK7">
         <v>2</v>
@@ -12071,6 +11968,9 @@
       <c r="AI8" s="7">
         <f t="shared" si="4"/>
         <v>6</v>
+      </c>
+      <c r="AJ8">
+        <v>2</v>
       </c>
       <c r="AK8">
         <v>2</v>
@@ -12131,7 +12031,7 @@
       <c r="BC8" s="19"/>
       <c r="BD8" s="19"/>
     </row>
-    <row r="9" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:65" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>92</v>
       </c>
@@ -12240,6 +12140,9 @@
       <c r="AI9" s="7">
         <f t="shared" si="4"/>
         <v>7</v>
+      </c>
+      <c r="AJ9">
+        <v>2</v>
       </c>
       <c r="AK9">
         <v>2</v>
@@ -12307,7 +12210,7 @@
       <c r="BH9" s="19"/>
       <c r="BI9" s="19"/>
     </row>
-    <row r="10" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:65" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>92</v>
       </c>
@@ -12417,6 +12320,9 @@
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
+      <c r="AJ10">
+        <v>2</v>
+      </c>
       <c r="AK10">
         <v>2</v>
       </c>
@@ -12475,7 +12381,7 @@
       </c>
       <c r="BA10" s="19"/>
     </row>
-    <row r="11" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:65" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>92</v>
       </c>
@@ -12584,6 +12490,9 @@
       <c r="AI11" s="7">
         <f t="shared" si="4"/>
         <v>5</v>
+      </c>
+      <c r="AJ11">
+        <v>2</v>
       </c>
       <c r="AK11">
         <v>2</v>
@@ -12641,7 +12550,7 @@
       <c r="BB11" s="19"/>
       <c r="BC11" s="19"/>
     </row>
-    <row r="12" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:65" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>92</v>
       </c>
@@ -12751,6 +12660,9 @@
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
+      <c r="AJ12">
+        <v>1</v>
+      </c>
       <c r="AK12">
         <v>1</v>
       </c>
@@ -12823,7 +12735,7 @@
         <v>79.186698913574219</v>
       </c>
     </row>
-    <row r="13" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:65" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>97</v>
       </c>
@@ -12933,6 +12845,9 @@
         <f t="shared" si="4"/>
         <v>10</v>
       </c>
+      <c r="AJ13">
+        <v>1</v>
+      </c>
       <c r="AK13">
         <v>1</v>
       </c>
@@ -12999,7 +12914,7 @@
         <v>65.188003540039063</v>
       </c>
     </row>
-    <row r="14" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:65" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>97</v>
       </c>
@@ -13109,6 +13024,9 @@
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
+      <c r="AJ14">
+        <v>2</v>
+      </c>
       <c r="AK14">
         <v>2</v>
       </c>
@@ -13163,7 +13081,7 @@
         <v>62.286701202392578</v>
       </c>
     </row>
-    <row r="15" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:65" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>97</v>
       </c>
@@ -13273,6 +13191,9 @@
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
+      <c r="AJ15">
+        <v>2</v>
+      </c>
       <c r="AK15">
         <v>2</v>
       </c>
@@ -13338,7 +13259,7 @@
       <c r="BC15" s="19"/>
       <c r="BD15" s="19"/>
     </row>
-    <row r="16" spans="1:65" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:65" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>97</v>
       </c>
@@ -13448,6 +13369,9 @@
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
+      <c r="AJ16">
+        <v>2</v>
+      </c>
       <c r="AK16">
         <v>2</v>
       </c>
@@ -13507,7 +13431,7 @@
       <c r="BA16" s="19"/>
       <c r="BB16" s="19"/>
     </row>
-    <row r="17" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:61" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>97</v>
       </c>
@@ -13618,6 +13542,9 @@
         <f t="shared" si="4"/>
         <v>11</v>
       </c>
+      <c r="AJ17">
+        <v>1</v>
+      </c>
       <c r="AK17">
         <v>1</v>
       </c>
@@ -13687,7 +13614,7 @@
         <v>144.052001953125</v>
       </c>
     </row>
-    <row r="18" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:61" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>97</v>
       </c>
@@ -13798,6 +13725,9 @@
         <f t="shared" si="4"/>
         <v>16</v>
       </c>
+      <c r="AJ18">
+        <v>1</v>
+      </c>
       <c r="AK18">
         <v>1</v>
       </c>
@@ -13882,7 +13812,7 @@
         <v>148.05000305175781</v>
       </c>
     </row>
-    <row r="19" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:61" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>97</v>
       </c>
@@ -13991,6 +13921,9 @@
       <c r="AI19" s="7">
         <f t="shared" si="4"/>
         <v>8</v>
+      </c>
+      <c r="AJ19">
+        <v>1</v>
       </c>
       <c r="AK19">
         <v>1</v>
@@ -14163,6 +14096,9 @@
         <f t="shared" si="4"/>
         <v>10</v>
       </c>
+      <c r="AJ20">
+        <v>2</v>
+      </c>
       <c r="AK20">
         <v>1</v>
       </c>
@@ -14339,6 +14275,9 @@
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
+      <c r="AJ21">
+        <v>2</v>
+      </c>
       <c r="AK21">
         <v>2</v>
       </c>
@@ -14506,6 +14445,9 @@
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
+      <c r="AJ22">
+        <v>2</v>
+      </c>
       <c r="AK22">
         <v>1</v>
       </c>
@@ -14571,7 +14513,7 @@
       <c r="BC22" s="19"/>
       <c r="BD22" s="19"/>
     </row>
-    <row r="23" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:61" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>97</v>
       </c>
@@ -14681,6 +14623,9 @@
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
+      <c r="AJ23">
+        <v>2</v>
+      </c>
       <c r="AK23">
         <v>2</v>
       </c>
@@ -14735,7 +14680,7 @@
         <v>166.031005859375</v>
       </c>
     </row>
-    <row r="24" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:61" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>97</v>
       </c>
@@ -14844,6 +14789,9 @@
       <c r="AI24" s="7">
         <f t="shared" si="4"/>
         <v>11</v>
+      </c>
+      <c r="AJ24">
+        <v>2</v>
       </c>
       <c r="AK24">
         <v>1</v>
@@ -15024,6 +14972,9 @@
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
+      <c r="AJ25">
+        <v>2</v>
+      </c>
       <c r="AK25">
         <v>1</v>
       </c>
@@ -15088,7 +15039,7 @@
       </c>
       <c r="BC25" s="19"/>
     </row>
-    <row r="26" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:61" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>97</v>
       </c>
@@ -15198,6 +15149,9 @@
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
+      <c r="AJ26">
+        <v>2</v>
+      </c>
       <c r="AK26">
         <v>2</v>
       </c>
@@ -15257,7 +15211,7 @@
       <c r="BA26" s="19"/>
       <c r="BB26" s="19"/>
     </row>
-    <row r="27" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:61" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>106</v>
       </c>
@@ -15367,6 +15321,9 @@
         <f t="shared" si="4"/>
         <v>11</v>
       </c>
+      <c r="AJ27">
+        <v>2</v>
+      </c>
       <c r="AK27">
         <v>1</v>
       </c>
@@ -15436,7 +15393,7 @@
         <v>133.68800354003906</v>
       </c>
     </row>
-    <row r="28" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:61" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>106</v>
       </c>
@@ -15546,6 +15503,9 @@
       <c r="AI28" s="7">
         <f t="shared" ref="AI28:AI33" si="10">SUM(AP28:AS28)</f>
         <v>9</v>
+      </c>
+      <c r="AJ28">
+        <v>2</v>
       </c>
       <c r="AK28">
         <v>2</v>
@@ -15720,6 +15680,9 @@
         <f t="shared" si="10"/>
         <v>6</v>
       </c>
+      <c r="AJ29">
+        <v>2</v>
+      </c>
       <c r="AK29">
         <v>2</v>
       </c>
@@ -15884,6 +15847,9 @@
         <f t="shared" si="10"/>
         <v>6</v>
       </c>
+      <c r="AJ30">
+        <v>2</v>
+      </c>
       <c r="AK30">
         <v>2</v>
       </c>
@@ -16048,6 +16014,9 @@
         <f t="shared" si="10"/>
         <v>6</v>
       </c>
+      <c r="AJ31">
+        <v>2</v>
+      </c>
       <c r="AK31">
         <v>2</v>
       </c>
@@ -16102,7 +16071,7 @@
         <v>120.04299926757812</v>
       </c>
     </row>
-    <row r="32" spans="1:61" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:61" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>106</v>
       </c>
@@ -16211,6 +16180,9 @@
       <c r="AI32" s="7">
         <f t="shared" si="10"/>
         <v>10</v>
+      </c>
+      <c r="AJ32">
+        <v>2</v>
       </c>
       <c r="AK32">
         <v>1</v>
@@ -16388,6 +16360,9 @@
         <f t="shared" si="10"/>
         <v>9</v>
       </c>
+      <c r="AJ33">
+        <v>2</v>
+      </c>
       <c r="AK33">
         <v>2</v>
       </c>
@@ -16454,7 +16429,7 @@
     <row r="34" spans="1:54" x14ac:dyDescent="0.25">
       <c r="AD34" s="13"/>
     </row>
-    <row r="35" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="E35" s="6">
         <f>SUMIF(E3:E33,1)</f>
         <v>10</v>
@@ -16472,7 +16447,7 @@
         <v>846.6</v>
       </c>
     </row>
-    <row r="36" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="E36" s="6">
         <f>SUMIF(E4:E34,2)/2</f>
         <v>12</v>
@@ -16490,7 +16465,7 @@
         <v>940.71428571428567</v>
       </c>
     </row>
-    <row r="37" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:54" hidden="1" x14ac:dyDescent="0.25">
       <c r="B37" s="24" t="s">
         <v>147</v>
       </c>
@@ -16552,8 +16527,68 @@
     <row r="43" spans="1:54" x14ac:dyDescent="0.25">
       <c r="AD43" s="13"/>
     </row>
+    <row r="45" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="AF45" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="AG45" s="7">
+        <v>1</v>
+      </c>
+      <c r="AH45" s="7">
+        <f>AVERAGE(AH5,AH8,AH20,AH21,AH22,AH25,AH30,AH29,AH31,AH33)</f>
+        <v>930.1</v>
+      </c>
+      <c r="AI45" s="13">
+        <f>AVERAGE(AI5,AI8,AI20,AI21,AI22,AI25,AI30,AI29,AI31,AI33)</f>
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="AF46" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="AG46" s="7">
+        <v>3</v>
+      </c>
+      <c r="AH46" s="7">
+        <f>AVERAGE(AH3,AH4,AH12,AH13,AH14,AH18,AH19,AH23,AH24)</f>
+        <v>821.77777777777783</v>
+      </c>
+      <c r="AI46" s="13">
+        <f>AVERAGE(AI3,AI4,AI12,AI13,AI14,AI18,AI19,AI23,AI24)</f>
+        <v>10.111111111111111</v>
+      </c>
+    </row>
+    <row r="47" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="AF47" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="AG47" s="7">
+        <v>2</v>
+      </c>
+      <c r="AH47" s="7">
+        <f>AVERAGE(AH6,AH7,AH9,AH10,AH11,AH15,AH16,AH17,AH26,AH27,AH28,AH32)</f>
+        <v>960.33333333333337</v>
+      </c>
+      <c r="AI47" s="13">
+        <f>AVERAGE(AI6,AI7,AI9,AI10,AI11,AI15,AI16,AI17,AI26,AI27,AI28,AI32)</f>
+        <v>8.4166666666666661</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:BM43"/>
+  <autoFilter ref="A1:BM43">
+    <filterColumn colId="4">
+      <filters blank="1">
+        <filter val="1"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="9">
+      <filters blank="1">
+        <filter val="3"/>
+        <filter val="4"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>

</xml_diff>